<commit_message>
Updated spreadsheet (episode 2)
</commit_message>
<xml_diff>
--- a/Performance Tracking.xlsx
+++ b/Performance Tracking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Version</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Test 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 5</t>
   </si>
   <si>
     <t xml:space="preserve">Average</t>
@@ -179,17 +182,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -231,16 +234,19 @@
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>8.28</v>
@@ -254,20 +260,20 @@
       <c r="G3" s="1" t="n">
         <v>8.12</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="I3" s="1" t="n">
         <f aca="false">AVERAGE(D3:G3)</f>
         <v>8.205</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>38.56</v>
@@ -282,8 +288,11 @@
         <v>30.28</v>
       </c>
       <c r="H4" s="1" t="n">
-        <f aca="false">AVERAGE(D4:G4)</f>
-        <v>31.03</v>
+        <v>76.08</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <f aca="false">AVERAGE(D4:H4)</f>
+        <v>40.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Used slightly modified Nvidia End-to-End Deep Learning model
</commit_message>
<xml_diff>
--- a/Performance Tracking.xlsx
+++ b/Performance Tracking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Version</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">1500310252.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1500327174.h5</t>
   </si>
 </sst>
 </file>
@@ -182,17 +185,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -208,6 +211,7 @@
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -260,6 +264,7 @@
       <c r="G3" s="1" t="n">
         <v>8.12</v>
       </c>
+      <c r="H3" s="0"/>
       <c r="I3" s="1" t="n">
         <f aca="false">AVERAGE(D3:G3)</f>
         <v>8.205</v>
@@ -293,6 +298,30 @@
       <c r="I4" s="1" t="n">
         <f aca="false">AVERAGE(D4:H4)</f>
         <v>40.04</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>9.74</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>7.94</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>8.62</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>7.58</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>7.82</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <f aca="false">AVERAGE(D5:H5)</f>
+        <v>8.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated spreadsheet -- success! It drives around the whole track!
</commit_message>
<xml_diff>
--- a/Performance Tracking.xlsx
+++ b/Performance Tracking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Version</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t xml:space="preserve">1500416566.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0915d0e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8bfdfc5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1500482174.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model successfully drives around entire track.</t>
   </si>
 </sst>
 </file>
@@ -203,18 +215,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.6122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -379,6 +391,20 @@
       <c r="I6" s="1" t="n">
         <f aca="false">AVERAGE(D6:H6)</f>
         <v>15.488</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>